<commit_message>
Google Sheets: Getting Started - GSP469
</commit_message>
<xml_diff>
--- a/labs/GSP469/important-data.xlsx
+++ b/labs/GSP469/important-data.xlsx
@@ -12,39 +12,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
-  <si>
-    <t>day</t>
-  </si>
-  <si>
-    <t>product</t>
-  </si>
-  <si>
-    <t>price</t>
-  </si>
-  <si>
-    <t>monday</t>
-  </si>
-  <si>
-    <t>pie</t>
-  </si>
-  <si>
-    <t>tuesday</t>
-  </si>
-  <si>
-    <t>wednesday</t>
-  </si>
-  <si>
-    <t>thursday</t>
-  </si>
-  <si>
-    <t>friday</t>
-  </si>
-  <si>
-    <t>saturday</t>
-  </si>
-  <si>
-    <t>sunday</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t># Sold</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Croissant</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Baguette</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Muffin</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Donut</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Cupcake</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>Bagel</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>Brownie</t>
   </si>
 </sst>
 </file>
@@ -315,93 +336,106 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1">
-        <v>10.0</v>
+        <v>2.5</v>
+      </c>
+      <c r="D2" s="1">
+        <v>120.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1">
-        <v>20.0</v>
+        <v>1.5</v>
+      </c>
+      <c r="D3" s="1">
+        <v>90.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1">
-        <v>30.0</v>
+        <v>2.0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>75.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1">
-        <v>40.0</v>
+        <v>1.8</v>
+      </c>
+      <c r="D5" s="1">
+        <v>130.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1">
-        <v>50.0</v>
+        <v>2.2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>110.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C7" s="1">
-        <v>20.0</v>
+        <v>1.7</v>
+      </c>
+      <c r="D7" s="1">
+        <v>95.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1">
-        <v>2060.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="1">
-        <v>20.0</v>
+        <v>2.8</v>
+      </c>
+      <c r="D8" s="1">
+        <v>100.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>